<commit_message>
Update plan's ARR and the preloaded choices
</commit_message>
<xml_diff>
--- a/Funding Model Inputs 2021.xlsx
+++ b/Funding Model Inputs 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongbui/Dropbox/Work/Reason/Reason Work/Montana/Benefit Models/Montana-PERS-BModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F668649-9778-664C-9BF5-7F73DAF28737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE17AE93-768A-C548-A265-4F1BCB7931B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1662,7 +1662,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1686,7 +1686,7 @@
         <v>215</v>
       </c>
       <c r="C2" s="25">
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1697,7 +1697,7 @@
         <v>216</v>
       </c>
       <c r="C3" s="25">
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1719,7 +1719,7 @@
         <v>258</v>
       </c>
       <c r="C5" s="13">
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4121,11 +4121,11 @@
       </c>
       <c r="D9" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E9" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F9" s="71">
         <v>-0.24</v>
@@ -4161,11 +4161,11 @@
       </c>
       <c r="D10" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E10" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F10" s="73">
         <v>0.11</v>
@@ -4201,11 +4201,11 @@
       </c>
       <c r="D11" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E11" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F11" s="73">
         <v>0.11</v>
@@ -4241,11 +4241,11 @@
       </c>
       <c r="D12" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E12" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F12" s="73">
         <v>0.11</v>
@@ -4281,11 +4281,11 @@
       </c>
       <c r="D13" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E13" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F13" s="74">
         <v>0.06</v>
@@ -4321,11 +4321,11 @@
       </c>
       <c r="D14" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E14" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F14" s="74">
         <v>0.06</v>
@@ -4361,11 +4361,11 @@
       </c>
       <c r="D15" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E15" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F15" s="74">
         <v>0.06</v>
@@ -4401,11 +4401,11 @@
       </c>
       <c r="D16" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E16" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F16" s="74">
         <v>0.06</v>
@@ -4441,11 +4441,11 @@
       </c>
       <c r="D17" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E17" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F17" s="74">
         <v>0.06</v>
@@ -4481,11 +4481,11 @@
       </c>
       <c r="D18" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E18" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F18" s="74">
         <v>0.06</v>
@@ -4521,11 +4521,11 @@
       </c>
       <c r="D19" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E19" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F19" s="74">
         <v>0.06</v>
@@ -4561,11 +4561,11 @@
       </c>
       <c r="D20" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E20" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F20" s="74">
         <v>0.06</v>
@@ -4601,11 +4601,11 @@
       </c>
       <c r="D21" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E21" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F21" s="74">
         <v>0.06</v>
@@ -4641,11 +4641,11 @@
       </c>
       <c r="D22" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E22" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F22" s="74">
         <v>0.06</v>
@@ -4681,11 +4681,11 @@
       </c>
       <c r="D23" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E23" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F23" s="74">
         <v>0.06</v>
@@ -4721,11 +4721,11 @@
       </c>
       <c r="D24" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E24" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F24" s="74">
         <v>0.06</v>
@@ -4761,11 +4761,11 @@
       </c>
       <c r="D25" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E25" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F25" s="74">
         <v>0.06</v>
@@ -4801,11 +4801,11 @@
       </c>
       <c r="D26" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E26" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F26" s="74">
         <v>0.06</v>
@@ -4841,11 +4841,11 @@
       </c>
       <c r="D27" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E27" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F27" s="74">
         <v>0.06</v>
@@ -4881,11 +4881,11 @@
       </c>
       <c r="D28" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E28" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F28" s="74">
         <v>0.06</v>
@@ -4921,11 +4921,11 @@
       </c>
       <c r="D29" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E29" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F29" s="74">
         <v>0.06</v>
@@ -4961,11 +4961,11 @@
       </c>
       <c r="D30" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E30" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F30" s="74">
         <v>0.06</v>
@@ -5001,11 +5001,11 @@
       </c>
       <c r="D31" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E31" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F31" s="74">
         <v>0.06</v>
@@ -5041,11 +5041,11 @@
       </c>
       <c r="D32" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E32" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F32" s="74">
         <v>0.06</v>
@@ -5081,11 +5081,11 @@
       </c>
       <c r="D33" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E33" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F33" s="74">
         <v>0.06</v>
@@ -5121,11 +5121,11 @@
       </c>
       <c r="D34" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E34" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F34" s="74">
         <v>0.06</v>
@@ -5161,11 +5161,11 @@
       </c>
       <c r="D35" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E35" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F35" s="74">
         <v>0.06</v>
@@ -5201,11 +5201,11 @@
       </c>
       <c r="D36" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E36" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F36" s="74">
         <v>0.06</v>
@@ -5241,11 +5241,11 @@
       </c>
       <c r="D37" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E37" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F37" s="74">
         <v>0.06</v>
@@ -5281,11 +5281,11 @@
       </c>
       <c r="D38" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E38" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F38" s="74">
         <v>0.06</v>
@@ -5321,11 +5321,11 @@
       </c>
       <c r="D39" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E39" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F39" s="74">
         <v>0.06</v>
@@ -5361,11 +5361,11 @@
       </c>
       <c r="D40" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E40" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F40" s="74">
         <v>0.06</v>
@@ -5401,11 +5401,11 @@
       </c>
       <c r="D41" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E41" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F41" s="74">
         <v>0.06</v>
@@ -5441,11 +5441,11 @@
       </c>
       <c r="D42" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E42" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F42" s="74">
         <v>0.06</v>
@@ -5481,11 +5481,11 @@
       </c>
       <c r="D43" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E43" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F43" s="74">
         <v>0.06</v>
@@ -5521,11 +5521,11 @@
       </c>
       <c r="D44" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E44" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F44" s="74">
         <v>0.06</v>
@@ -5561,11 +5561,11 @@
       </c>
       <c r="D45" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E45" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F45" s="74">
         <v>0.06</v>
@@ -5601,11 +5601,11 @@
       </c>
       <c r="D46" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E46" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F46" s="74">
         <v>0.06</v>
@@ -5641,11 +5641,11 @@
       </c>
       <c r="D47" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E47" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F47" s="74">
         <v>0.06</v>
@@ -5681,11 +5681,11 @@
       </c>
       <c r="D48" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E48" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F48" s="74">
         <v>0.06</v>
@@ -5721,11 +5721,11 @@
       </c>
       <c r="D49" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E49" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F49" s="74">
         <v>0.06</v>
@@ -5761,11 +5761,11 @@
       </c>
       <c r="D50" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E50" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F50" s="74">
         <v>0.06</v>
@@ -5801,11 +5801,11 @@
       </c>
       <c r="D51" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E51" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F51" s="74">
         <v>0.06</v>
@@ -5841,11 +5841,11 @@
       </c>
       <c r="D52" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E52" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F52" s="74">
         <v>0.06</v>
@@ -5881,11 +5881,11 @@
       </c>
       <c r="D53" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E53" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F53" s="74">
         <v>0.06</v>
@@ -5921,11 +5921,11 @@
       </c>
       <c r="D54" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E54" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F54" s="74">
         <v>0.06</v>
@@ -5961,11 +5961,11 @@
       </c>
       <c r="D55" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E55" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F55" s="74">
         <v>0.06</v>
@@ -6001,11 +6001,11 @@
       </c>
       <c r="D56" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E56" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F56" s="74">
         <v>0.06</v>
@@ -6041,11 +6041,11 @@
       </c>
       <c r="D57" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E57" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F57" s="74">
         <v>0.06</v>
@@ -6081,11 +6081,11 @@
       </c>
       <c r="D58" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E58" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F58" s="74">
         <v>0.06</v>
@@ -6121,11 +6121,11 @@
       </c>
       <c r="D59" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E59" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F59" s="74">
         <v>0.06</v>
@@ -6161,11 +6161,11 @@
       </c>
       <c r="D60" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E60" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F60" s="74">
         <v>0.06</v>
@@ -6201,11 +6201,11 @@
       </c>
       <c r="D61" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E61" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F61" s="74">
         <v>0.06</v>
@@ -6241,11 +6241,11 @@
       </c>
       <c r="D62" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E62" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F62" s="74">
         <v>0.06</v>
@@ -6281,11 +6281,11 @@
       </c>
       <c r="D63" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E63" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F63" s="74">
         <v>0.06</v>
@@ -6321,11 +6321,11 @@
       </c>
       <c r="D64" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E64" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F64" s="74">
         <v>0.06</v>
@@ -6361,11 +6361,11 @@
       </c>
       <c r="D65" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E65" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F65" s="74">
         <v>0.06</v>
@@ -6401,11 +6401,11 @@
       </c>
       <c r="D66" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E66" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F66" s="74">
         <v>0.06</v>
@@ -6441,11 +6441,11 @@
       </c>
       <c r="D67" s="69">
         <f>'Numeric Inputs'!$C$5</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E67" s="70">
         <f>'Numeric Inputs'!$C$2</f>
-        <v>7.6499999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F67" s="74">
         <v>0.06</v>

</xml_diff>

<commit_message>
Updare 2022 return and temporarily revise the return index
</commit_message>
<xml_diff>
--- a/Funding Model Inputs 2021.xlsx
+++ b/Funding Model Inputs 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongbui/Dropbox/Work/Reason/Reason Work/Montana/Benefit Models/Montana-PERS-BModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE17AE93-768A-C548-A265-4F1BCB7931B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD4428D-C5E1-6047-876F-3C1AB629C015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeric Inputs" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="Historical Data" sheetId="2" r:id="rId7"/>
     <sheet name="Benefit Payments" sheetId="11" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <calcPr calcId="191029" calcMode="autoNoTable"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -857,7 +860,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -865,6 +868,7 @@
     <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="#,##0.0_);\(#,##0.0\)"/>
+    <numFmt numFmtId="170" formatCode="0.000000000000000%"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1113,7 +1117,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1372,6 +1376,7 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1394,6 +1399,44 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Numeric Inputs"/>
+      <sheetName val="Character Inputs"/>
+      <sheetName val="List Box"/>
+      <sheetName val="Amortization_NewDebt"/>
+      <sheetName val="Amortization_CurrentDebt"/>
+      <sheetName val="Inv_Returns"/>
+      <sheetName val="Historical Data"/>
+      <sheetName val="Benefit Payments"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="C2">
+            <v>7.2999999999999995E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>7.2999999999999995E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1661,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1713,8 @@
     <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2213,7 +2257,7 @@
         <v>78</v>
       </c>
       <c r="C47" s="65">
-        <v>8.3366394042968806E-2</v>
+        <v>7.9888164348844645E-2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2226,6 +2270,7 @@
       <c r="C48" s="66">
         <v>6.9290149999999995E-2</v>
       </c>
+      <c r="E48" s="106"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -3787,8 +3832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4120,18 +4165,16 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D9" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="E9" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="F9" s="71">
-        <v>-0.24</v>
-      </c>
-      <c r="G9" s="71">
-        <v>-0.24</v>
+        <v>-4.3999999999999997E-2</v>
+      </c>
+      <c r="E9" s="69">
+        <v>-4.3999999999999997E-2</v>
+      </c>
+      <c r="F9" s="69">
+        <v>-4.3999999999999997E-2</v>
+      </c>
+      <c r="G9" s="69">
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="H9" s="72">
         <v>0.05</v>
@@ -4160,18 +4203,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D10" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E10" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="F10" s="73">
-        <v>0.11</v>
-      </c>
-      <c r="G10" s="73">
-        <v>0.11</v>
+        <f>'[1]Numeric Inputs'!$C$2</f>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F10" s="71">
+        <v>-0.24</v>
+      </c>
+      <c r="G10" s="71">
+        <v>-0.24</v>
       </c>
       <c r="H10" s="72">
         <v>0.05</v>
@@ -4200,11 +4243,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D11" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E11" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F11" s="73">
@@ -4240,11 +4283,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D12" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E12" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F12" s="73">
@@ -4280,18 +4323,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D13" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E13" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="F13" s="74">
-        <v>0.06</v>
-      </c>
-      <c r="G13" s="74">
-        <v>0.06</v>
+        <f>'[1]Numeric Inputs'!$C$2</f>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F13" s="73">
+        <v>0.11</v>
+      </c>
+      <c r="G13" s="73">
+        <v>0.11</v>
       </c>
       <c r="H13" s="72">
         <v>0.05</v>
@@ -4320,11 +4363,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D14" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E14" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F14" s="74">
@@ -4360,11 +4403,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D15" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E15" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F15" s="74">
@@ -4400,11 +4443,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D16" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E16" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F16" s="74">
@@ -4440,11 +4483,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D17" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E17" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F17" s="74">
@@ -4480,11 +4523,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D18" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E18" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F18" s="74">
@@ -4520,11 +4563,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D19" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E19" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F19" s="74">
@@ -4560,11 +4603,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D20" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E20" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F20" s="74">
@@ -4600,11 +4643,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D21" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E21" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F21" s="74">
@@ -4640,11 +4683,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D22" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E22" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F22" s="74">
@@ -4680,11 +4723,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D23" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E23" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F23" s="74">
@@ -4720,18 +4763,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D24" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E24" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F24" s="74">
         <v>0.06</v>
       </c>
-      <c r="G24" s="73">
-        <v>-0.24</v>
+      <c r="G24" s="74">
+        <v>0.06</v>
       </c>
       <c r="H24" s="75">
         <v>8.0142406836996249E-2</v>
@@ -4760,18 +4803,18 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D25" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E25" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F25" s="74">
         <v>0.06</v>
       </c>
       <c r="G25" s="73">
-        <v>0.11</v>
+        <v>-0.24</v>
       </c>
       <c r="H25" s="75">
         <v>8.0142406836996249E-2</v>
@@ -4800,11 +4843,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D26" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E26" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F26" s="74">
@@ -4840,11 +4883,11 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="D27" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E27" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F27" s="74">
@@ -4880,18 +4923,18 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="D28" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E28" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F28" s="74">
         <v>0.06</v>
       </c>
-      <c r="G28" s="74">
-        <v>0.06</v>
+      <c r="G28" s="73">
+        <v>0.11</v>
       </c>
       <c r="H28" s="75">
         <v>8.0142406836996249E-2</v>
@@ -4920,11 +4963,11 @@
         <v>0.02</v>
       </c>
       <c r="D29" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E29" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F29" s="74">
@@ -4960,11 +5003,11 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="D30" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E30" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F30" s="74">
@@ -5000,11 +5043,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="D31" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E31" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F31" s="74">
@@ -5040,11 +5083,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D32" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E32" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F32" s="74">
@@ -5080,11 +5123,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D33" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E33" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F33" s="74">
@@ -5120,11 +5163,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D34" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E34" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F34" s="74">
@@ -5160,11 +5203,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D35" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E35" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F35" s="74">
@@ -5200,11 +5243,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D36" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E36" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F36" s="74">
@@ -5240,11 +5283,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D37" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E37" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F37" s="74">
@@ -5280,11 +5323,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D38" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E38" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F38" s="74">
@@ -5320,11 +5363,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D39" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E39" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F39" s="74">
@@ -5360,11 +5403,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D40" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E40" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F40" s="74">
@@ -5400,11 +5443,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D41" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E41" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F41" s="74">
@@ -5440,11 +5483,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D42" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E42" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F42" s="74">
@@ -5480,11 +5523,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D43" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E43" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F43" s="74">
@@ -5520,11 +5563,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D44" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E44" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F44" s="74">
@@ -5560,11 +5603,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D45" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E45" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F45" s="74">
@@ -5600,11 +5643,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D46" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E46" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F46" s="74">
@@ -5640,11 +5683,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D47" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E47" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F47" s="74">
@@ -5680,11 +5723,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D48" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E48" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F48" s="74">
@@ -5720,11 +5763,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D49" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E49" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F49" s="74">
@@ -5760,11 +5803,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D50" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E50" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F50" s="74">
@@ -5800,11 +5843,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D51" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E51" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F51" s="74">
@@ -5840,11 +5883,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D52" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E52" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F52" s="74">
@@ -5880,11 +5923,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D53" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E53" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F53" s="74">
@@ -5920,11 +5963,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D54" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E54" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F54" s="74">
@@ -5960,11 +6003,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D55" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E55" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F55" s="74">
@@ -6000,11 +6043,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D56" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E56" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F56" s="74">
@@ -6040,11 +6083,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D57" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E57" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F57" s="74">
@@ -6080,11 +6123,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D58" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E58" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F58" s="74">
@@ -6120,11 +6163,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D59" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E59" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F59" s="74">
@@ -6160,11 +6203,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D60" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E60" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F60" s="74">
@@ -6200,11 +6243,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D61" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E61" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F61" s="74">
@@ -6240,11 +6283,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D62" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E62" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F62" s="74">
@@ -6280,11 +6323,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D63" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E63" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F63" s="74">
@@ -6320,11 +6363,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D64" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E64" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F64" s="74">
@@ -6360,11 +6403,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D65" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E65" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F65" s="74">
@@ -6400,11 +6443,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D66" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E66" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F66" s="74">
@@ -6440,11 +6483,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D67" s="69">
-        <f>'Numeric Inputs'!$C$5</f>
+        <f>'[1]Numeric Inputs'!$C$5</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E67" s="70">
-        <f>'Numeric Inputs'!$C$2</f>
+        <f>'[1]Numeric Inputs'!$C$2</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F67" s="74">
@@ -6478,7 +6521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CZ13"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AV8" sqref="AV8"/>
     </sheetView>
   </sheetViews>

</xml_diff>